<commit_message>
adding filters for owner advance
</commit_message>
<xml_diff>
--- a/src/containers/Onboarding/ONBOARDING-OWNERMASTER-TEMPLATE.xlsx
+++ b/src/containers/Onboarding/ONBOARDING-OWNERMASTER-TEMPLATE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AIVOLVED-JOB\TRUCKLINK-UI\git\new-backend-ekfrazo\trucklinkold\app\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AIVOLVED-JOB\TRUCKLINK-UI\trucklink-frontend\src\containers\Onboarding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76078CAA-7913-45B8-B824-23D259376828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546CEF96-75BD-4C89-8A95-102B333BC863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{CBD8B912-6A71-4E18-8F60-F0983606B247}"/>
   </bookViews>
@@ -2376,9 +2376,6 @@
     <t>cnrb</t>
   </si>
   <si>
-    <t>66541b73a74686d081580179</t>
-  </si>
-  <si>
     <t>ttaayyiibb</t>
   </si>
   <si>
@@ -2386,13 +2383,16 @@
   </si>
   <si>
     <t>ttaayyiibb987651</t>
+  </si>
+  <si>
+    <t>6672c64da1f599d68bf6a4ce</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2423,6 +2423,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF161D1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2445,7 +2451,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -2458,6 +2464,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2775,16 +2782,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC97E9D5-212A-430B-8394-0484CA5C8F42}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="31.109375" customWidth="1"/>
-    <col min="5" max="5" width="27.88671875" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -2833,31 +2842,31 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D2" t="s">
         <v>739</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="G2">
         <v>9550995582</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="I2">
         <v>955409879556</v>
       </c>
       <c r="J2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="K2" t="s">
         <v>763</v>
@@ -2868,8 +2877,8 @@
       <c r="M2" t="s">
         <v>764</v>
       </c>
-      <c r="N2" t="s">
-        <v>765</v>
+      <c r="N2" s="8" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -2895,8 +2904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1902DD6E-459A-48E1-BF1D-61581B61F496}">
   <dimension ref="A1:AL77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>